<commit_message>
completa datapackage, reorganiza e renomeia arquivos divida
</commit_message>
<xml_diff>
--- a/metadados-depara.xlsx
+++ b/metadados-depara.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="101">
   <si>
     <t>FRICTIONLESS_DATA</t>
   </si>
@@ -87,9 +87,6 @@
     <t xml:space="preserve"> a description of the dataset (optional)</t>
   </si>
   <si>
-    <t>homepage</t>
-  </si>
-  <si>
     <t>url </t>
   </si>
   <si>
@@ -271,6 +268,60 @@
   </si>
   <si>
     <t>https://specs.frictionlessdata.io/data-package/#specification</t>
+  </si>
+  <si>
+    <t>homepage/path</t>
+  </si>
+  <si>
+    <t>package_id </t>
+  </si>
+  <si>
+    <t>revision_id </t>
+  </si>
+  <si>
+    <t>description </t>
+  </si>
+  <si>
+    <t>format </t>
+  </si>
+  <si>
+    <t>hash </t>
+  </si>
+  <si>
+    <t>resource_type </t>
+  </si>
+  <si>
+    <t>mimetype </t>
+  </si>
+  <si>
+    <t>mimetype_inner </t>
+  </si>
+  <si>
+    <t>cache_url </t>
+  </si>
+  <si>
+    <t>size </t>
+  </si>
+  <si>
+    <t>created </t>
+  </si>
+  <si>
+    <t>last_modified </t>
+  </si>
+  <si>
+    <t>cache_last_updated </t>
+  </si>
+  <si>
+    <t>upload </t>
+  </si>
+  <si>
+    <t>FieldStorage </t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>iso date string</t>
   </si>
 </sst>
 </file>
@@ -600,7 +651,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -733,6 +784,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -778,7 +838,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -787,6 +847,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1108,11 +1169,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,306 +1269,466 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="D24" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="5"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="5"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B49" t="s">
         <v>80</v>
       </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>